<commit_message>
small typos in MAX7317 messages
</commit_message>
<xml_diff>
--- a/hk_command_deck.xlsx
+++ b/hk_command_deck.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thanasi/Documents/FOXSI/Data/formatter/foxsi4-commands/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED1BB236-C29F-E44B-AE73-365F0E6E1A48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E594456F-4B9F-C244-A244-8721539DD697}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17920" xr2:uid="{1DE950B2-129E-5A4D-8896-FB78BBCF4CAC}"/>
   </bookViews>
@@ -799,10 +799,10 @@
   <dimension ref="A1:AC38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="L3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AA33" sqref="AA33"/>
+      <selection pane="bottomRight" activeCell="Y5" sqref="Y5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.25"/>
@@ -1121,7 +1121,7 @@
         <v>48</v>
       </c>
       <c r="Y4" s="22" t="s">
-        <v>56</v>
+        <v>81</v>
       </c>
       <c r="Z4" s="3" t="s">
         <v>96</v>
@@ -1211,7 +1211,7 @@
         <v>48</v>
       </c>
       <c r="Y5" s="22" t="s">
-        <v>56</v>
+        <v>81</v>
       </c>
       <c r="Z5" s="3" t="s">
         <v>83</v>

</xml_diff>